<commit_message>
first working alpha version of JEBT, with XLSX and inner loops.
</commit_message>
<xml_diff>
--- a/src/test/resources/xlsx/basicXlsxTemplateResult.xlsx
+++ b/src/test/resources/xlsx/basicXlsxTemplateResult.xlsx
@@ -31,10 +31,10 @@
     <t>Even with Text formatting: Some bold World! But only the cell font will be preserved. Any text-section specific formatting will be discarded.</t>
   </si>
   <si>
+    <t>World folks, Let Jebt take on the World</t>
+  </si>
+  <si>
     <t>The postal code of the third customer is 200093.</t>
-  </si>
-  <si>
-    <t>World folks, Let Jebt take on the World</t>
   </si>
 </sst>
 </file>
@@ -398,7 +398,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,7 +425,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -435,7 +435,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="F9" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>